<commit_message>
Progress to final stage ... but style some bugs difficult to fix
</commit_message>
<xml_diff>
--- a/ressources/Tableau-Gaz-pression-temp.xlsx
+++ b/ressources/Tableau-Gaz-pression-temp.xlsx
@@ -4,17 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="15" windowWidth="18960" windowHeight="11325"/>
+    <workbookView xWindow="120" yWindow="15" windowWidth="18960" windowHeight="11325" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Table 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Press-Temp" sheetId="1" r:id="rId1"/>
+    <sheet name="R22" sheetId="3" r:id="rId2"/>
+    <sheet name="Feuil2" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" calcMode="manual" calcCompleted="0" calcOnSave="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t>R-410A</t>
   </si>
@@ -146,6 +148,49 @@
   <si>
     <t>Il faut ajouter 1bar au pression ci-dessous, pour avoir la valeur sur le tableau enthalpique</t>
   </si>
+  <si>
+    <t>Presssure
+(MPa)</t>
+  </si>
+  <si>
+    <t>Liquid Density
+(kg/m3)</t>
+  </si>
+  <si>
+    <t>Vapor Volume
+(m3/kg)</t>
+  </si>
+  <si>
+    <t>Temperature
+(°C)</t>
+  </si>
+  <si>
+    <t>http://www.engineeringtoolbox.com/r22-properties-d_365.html</t>
+  </si>
+  <si>
+    <t>Enthalpy
+(kJ/kg)
+Liquid</t>
+  </si>
+  <si>
+    <t>Enthalpy
+(kJ/kg)
+Vapor</t>
+  </si>
+  <si>
+    <t>Entropy
+(kJ/kgK)
+Liquid</t>
+  </si>
+  <si>
+    <t>Entropy
+(kJ/kgK)
+Vapor</t>
+  </si>
+  <si>
+    <t>Pressure
+Absolute</t>
+  </si>
 </sst>
 </file>
 
@@ -160,7 +205,7 @@
     <numFmt numFmtId="169" formatCode="#,##0;#,##0"/>
     <numFmt numFmtId="170" formatCode="###0.0;###0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -197,16 +242,74 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor theme="7" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor theme="7" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor theme="7"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -319,11 +422,88 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -417,11 +597,243 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="32">
+  <dxfs count="43">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1344,43 +1756,63 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A2:M57" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A2:M57" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
   <autoFilter ref="A2:M57"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="Temp Cº    " dataDxfId="29"/>
-    <tableColumn id="2" name="R-22_x000a_(bar_x000a_relatif)" dataDxfId="28"/>
-    <tableColumn id="3" name="R-417A _x000a_(I-59)_x000a_Líquide" dataDxfId="27"/>
-    <tableColumn id="4" name="R-417A _x000a_(I-59)_x000a_Vapeur" dataDxfId="26"/>
-    <tableColumn id="5" name="R-424A _x000a_(RS-44)_x000a_Líquide" dataDxfId="25"/>
-    <tableColumn id="6" name="R-424A_x000a_ (RS-44)_x000a_Vapeur" dataDxfId="24"/>
-    <tableColumn id="7" name="R-422D _x000a_(I-29)_x000a_Líquide" dataDxfId="23"/>
-    <tableColumn id="8" name="R-422D _x000a_(I-29)_x000a_Vapeur" dataDxfId="22"/>
-    <tableColumn id="9" name="R-434A _x000a_(RS-45)_x000a_Líquide" dataDxfId="21"/>
-    <tableColumn id="10" name="R-434A _x000a_(RS-45)_x000a_Vapeur" dataDxfId="20"/>
-    <tableColumn id="11" name="R-407C_x000a_Líquide" dataDxfId="19"/>
-    <tableColumn id="12" name="R-407C_x000a_Vapeur" dataDxfId="18"/>
-    <tableColumn id="13" name="R-410A" dataDxfId="17"/>
+    <tableColumn id="1" name="Temp Cº    " dataDxfId="40"/>
+    <tableColumn id="2" name="R-22_x000a_(bar_x000a_relatif)" dataDxfId="39"/>
+    <tableColumn id="3" name="R-417A _x000a_(I-59)_x000a_Líquide" dataDxfId="38"/>
+    <tableColumn id="4" name="R-417A _x000a_(I-59)_x000a_Vapeur" dataDxfId="37"/>
+    <tableColumn id="5" name="R-424A _x000a_(RS-44)_x000a_Líquide" dataDxfId="36"/>
+    <tableColumn id="6" name="R-424A_x000a_ (RS-44)_x000a_Vapeur" dataDxfId="35"/>
+    <tableColumn id="7" name="R-422D _x000a_(I-29)_x000a_Líquide" dataDxfId="34"/>
+    <tableColumn id="8" name="R-422D _x000a_(I-29)_x000a_Vapeur" dataDxfId="33"/>
+    <tableColumn id="9" name="R-434A _x000a_(RS-45)_x000a_Líquide" dataDxfId="32"/>
+    <tableColumn id="10" name="R-434A _x000a_(RS-45)_x000a_Vapeur" dataDxfId="31"/>
+    <tableColumn id="11" name="R-407C_x000a_Líquide" dataDxfId="30"/>
+    <tableColumn id="12" name="R-407C_x000a_Vapeur" dataDxfId="29"/>
+    <tableColumn id="13" name="R-410A" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A61:L116" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13" totalsRowBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tableau2" displayName="Tableau2" ref="A61:L116" totalsRowShown="0" headerRowDxfId="27" dataDxfId="25" headerRowBorderDxfId="26" tableBorderDxfId="24" totalsRowBorderDxfId="23">
   <autoFilter ref="A61:L116"/>
   <tableColumns count="12">
-    <tableColumn id="1" name="Temp Cº" dataDxfId="11"/>
-    <tableColumn id="2" name="R-422A _x000a_(I-79)_x000a_Líquido" dataDxfId="10"/>
-    <tableColumn id="3" name="R-422A _x000a_(I-79)_x000a_Vapor" dataDxfId="9"/>
-    <tableColumn id="4" name="R-428A _x000a_(RS-52)_x000a_Líquido" dataDxfId="8"/>
-    <tableColumn id="5" name="R-428A _x000a_(RS-52)_x000a_Vapor" dataDxfId="7"/>
-    <tableColumn id="6" name="R-404A" dataDxfId="6"/>
-    <tableColumn id="7" name="R-507" dataDxfId="5"/>
-    <tableColumn id="8" name="R-442A _x000a_(RS-50)_x000a_Líquido" dataDxfId="4"/>
-    <tableColumn id="9" name="R-442A _x000a_(RS-50)_x000a_Vapor" dataDxfId="3"/>
-    <tableColumn id="10" name="R-134a" dataDxfId="2"/>
-    <tableColumn id="11" name="R-426A _x000a_(RS-24)_x000a_Líquido" dataDxfId="1"/>
-    <tableColumn id="12" name="R-426A _x000a_(RS-24)_x000a_Vapor" dataDxfId="0"/>
+    <tableColumn id="1" name="Temp Cº" dataDxfId="22"/>
+    <tableColumn id="2" name="R-422A _x000a_(I-79)_x000a_Líquido" dataDxfId="21"/>
+    <tableColumn id="3" name="R-422A _x000a_(I-79)_x000a_Vapor" dataDxfId="20"/>
+    <tableColumn id="4" name="R-428A _x000a_(RS-52)_x000a_Líquido" dataDxfId="19"/>
+    <tableColumn id="5" name="R-428A _x000a_(RS-52)_x000a_Vapor" dataDxfId="18"/>
+    <tableColumn id="6" name="R-404A" dataDxfId="17"/>
+    <tableColumn id="7" name="R-507" dataDxfId="16"/>
+    <tableColumn id="8" name="R-442A _x000a_(RS-50)_x000a_Líquido" dataDxfId="15"/>
+    <tableColumn id="9" name="R-442A _x000a_(RS-50)_x000a_Vapor" dataDxfId="14"/>
+    <tableColumn id="10" name="R-134a" dataDxfId="13"/>
+    <tableColumn id="11" name="R-426A _x000a_(RS-24)_x000a_Líquido" dataDxfId="12"/>
+    <tableColumn id="12" name="R-426A _x000a_(RS-24)_x000a_Vapor" dataDxfId="11"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tableau3" displayName="Tableau3" ref="B3:J70" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="B3:J70"/>
+  <tableColumns count="9">
+    <tableColumn id="1" name="Temperature_x000a_(°C)" dataDxfId="8"/>
+    <tableColumn id="2" name="Presssure_x000a_(MPa)" dataDxfId="7"/>
+    <tableColumn id="3" name="Pressure_x000a_Absolute" dataDxfId="6">
+      <calculatedColumnFormula>C4*10</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" name="Liquid Density_x000a_(kg/m3)" dataDxfId="5"/>
+    <tableColumn id="5" name="Vapor Volume_x000a_(m3/kg)" dataDxfId="4"/>
+    <tableColumn id="6" name="Enthalpy_x000a_(kJ/kg)_x000a_Liquid" dataDxfId="3"/>
+    <tableColumn id="7" name="Enthalpy_x000a_(kJ/kg)_x000a_Vapor" dataDxfId="2"/>
+    <tableColumn id="8" name="Entropy_x000a_(kJ/kgK)_x000a_Liquid" dataDxfId="1"/>
+    <tableColumn id="9" name="Entropy_x000a_(kJ/kgK)_x000a_Vapor" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1675,8 +2107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M116"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D119" sqref="D119"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1686,7 +2118,7 @@
     <col min="24" max="16384" width="9.33203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>25</v>
       </c>
@@ -3998,7 +4430,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="61" spans="1:13" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13" ht="45" x14ac:dyDescent="0.2">
       <c r="A61" s="21" t="s">
         <v>1</v>
       </c>
@@ -6124,4 +6556,2944 @@
     <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J70"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:D70"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8.5" style="33" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" style="33" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" style="33" customWidth="1"/>
+    <col min="4" max="4" width="15" style="33" customWidth="1"/>
+    <col min="5" max="5" width="16.5" style="33" customWidth="1"/>
+    <col min="6" max="6" width="14" style="33" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" style="33" customWidth="1"/>
+    <col min="8" max="10" width="14.6640625" style="33" customWidth="1"/>
+    <col min="11" max="16384" width="12" style="33"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B1" s="35" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="35"/>
+    </row>
+    <row r="3" spans="1:10" s="34" customFormat="1" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="33">
+        <v>0</v>
+      </c>
+      <c r="B4" s="31">
+        <v>-100</v>
+      </c>
+      <c r="C4" s="31">
+        <v>2E-3</v>
+      </c>
+      <c r="D4" s="31">
+        <f t="shared" ref="D4:D35" si="0">C4*10</f>
+        <v>0.02</v>
+      </c>
+      <c r="E4" s="31">
+        <v>1571.7</v>
+      </c>
+      <c r="F4" s="31">
+        <v>8.298</v>
+      </c>
+      <c r="G4" s="31">
+        <v>90.24</v>
+      </c>
+      <c r="H4" s="31">
+        <v>358.93</v>
+      </c>
+      <c r="I4" s="31">
+        <v>0.50270000000000004</v>
+      </c>
+      <c r="J4" s="31">
+        <v>2.0545</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="33">
+        <v>1</v>
+      </c>
+      <c r="B5" s="31">
+        <v>-90</v>
+      </c>
+      <c r="C5" s="31">
+        <v>4.7999999999999996E-3</v>
+      </c>
+      <c r="D5" s="31">
+        <f t="shared" si="0"/>
+        <v>4.7999999999999994E-2</v>
+      </c>
+      <c r="E5" s="31">
+        <v>1545.1</v>
+      </c>
+      <c r="F5" s="31">
+        <v>3.6547999999999998</v>
+      </c>
+      <c r="G5" s="31">
+        <v>100.95</v>
+      </c>
+      <c r="H5" s="31">
+        <v>363.82</v>
+      </c>
+      <c r="I5" s="31">
+        <v>0.56289999999999996</v>
+      </c>
+      <c r="J5" s="31">
+        <v>1.9982</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="33">
+        <v>2</v>
+      </c>
+      <c r="B6" s="31">
+        <v>-80</v>
+      </c>
+      <c r="C6" s="31">
+        <v>1.035E-2</v>
+      </c>
+      <c r="D6" s="31">
+        <f t="shared" si="0"/>
+        <v>0.10349999999999999</v>
+      </c>
+      <c r="E6" s="31">
+        <v>1518.3</v>
+      </c>
+      <c r="F6" s="31">
+        <v>1.7816000000000001</v>
+      </c>
+      <c r="G6" s="31">
+        <v>111.66</v>
+      </c>
+      <c r="H6" s="31">
+        <v>368.75</v>
+      </c>
+      <c r="I6" s="31">
+        <v>0.61970000000000003</v>
+      </c>
+      <c r="J6" s="31">
+        <v>1.9508000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="33">
+        <v>3</v>
+      </c>
+      <c r="B7" s="31">
+        <v>-70</v>
+      </c>
+      <c r="C7" s="31">
+        <v>2.044E-2</v>
+      </c>
+      <c r="D7" s="31">
+        <f t="shared" si="0"/>
+        <v>0.2044</v>
+      </c>
+      <c r="E7" s="31">
+        <v>1491.1</v>
+      </c>
+      <c r="F7" s="31">
+        <v>0.94476000000000004</v>
+      </c>
+      <c r="G7" s="31">
+        <v>122.36</v>
+      </c>
+      <c r="H7" s="31">
+        <v>373.68</v>
+      </c>
+      <c r="I7" s="31">
+        <v>0.67379999999999995</v>
+      </c>
+      <c r="J7" s="31">
+        <v>1.9109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="33">
+        <v>4</v>
+      </c>
+      <c r="B8" s="31">
+        <v>-60</v>
+      </c>
+      <c r="C8" s="31">
+        <v>3.7470000000000003E-2</v>
+      </c>
+      <c r="D8" s="31">
+        <f t="shared" si="0"/>
+        <v>0.37470000000000003</v>
+      </c>
+      <c r="E8" s="31">
+        <v>1463.6</v>
+      </c>
+      <c r="F8" s="31">
+        <v>0.53734000000000004</v>
+      </c>
+      <c r="G8" s="31">
+        <v>133.11000000000001</v>
+      </c>
+      <c r="H8" s="31">
+        <v>378.58</v>
+      </c>
+      <c r="I8" s="31">
+        <v>0.72529999999999994</v>
+      </c>
+      <c r="J8" s="31">
+        <v>1.877</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="33">
+        <v>5</v>
+      </c>
+      <c r="B9" s="31">
+        <v>-50</v>
+      </c>
+      <c r="C9" s="31">
+        <v>6.4490000000000006E-2</v>
+      </c>
+      <c r="D9" s="31">
+        <f t="shared" si="0"/>
+        <v>0.64490000000000003</v>
+      </c>
+      <c r="E9" s="31">
+        <v>1435.5</v>
+      </c>
+      <c r="F9" s="31">
+        <v>0.32405</v>
+      </c>
+      <c r="G9" s="31">
+        <v>143.91</v>
+      </c>
+      <c r="H9" s="31">
+        <v>383.39</v>
+      </c>
+      <c r="I9" s="31">
+        <v>0.77480000000000004</v>
+      </c>
+      <c r="J9" s="31">
+        <v>1.8480000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="33">
+        <v>6</v>
+      </c>
+      <c r="B10" s="31">
+        <v>-48</v>
+      </c>
+      <c r="C10" s="31">
+        <v>7.1400000000000005E-2</v>
+      </c>
+      <c r="D10" s="31">
+        <f t="shared" si="0"/>
+        <v>0.71400000000000008</v>
+      </c>
+      <c r="E10" s="31">
+        <v>1429.8</v>
+      </c>
+      <c r="F10" s="31">
+        <v>0.29469000000000001</v>
+      </c>
+      <c r="G10" s="31">
+        <v>146.08000000000001</v>
+      </c>
+      <c r="H10" s="31">
+        <v>384.35</v>
+      </c>
+      <c r="I10" s="31">
+        <v>0.78439999999999999</v>
+      </c>
+      <c r="J10" s="31">
+        <v>1.8427</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="33">
+        <v>7</v>
+      </c>
+      <c r="B11" s="31">
+        <v>-46</v>
+      </c>
+      <c r="C11" s="31">
+        <v>7.8899999999999998E-2</v>
+      </c>
+      <c r="D11" s="31">
+        <f t="shared" si="0"/>
+        <v>0.78899999999999992</v>
+      </c>
+      <c r="E11" s="31">
+        <v>1424.1</v>
+      </c>
+      <c r="F11" s="31">
+        <v>0.26849000000000001</v>
+      </c>
+      <c r="G11" s="31">
+        <v>148.25</v>
+      </c>
+      <c r="H11" s="31">
+        <v>385.29</v>
+      </c>
+      <c r="I11" s="31">
+        <v>0.79400000000000004</v>
+      </c>
+      <c r="J11" s="31">
+        <v>1.8375999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="33">
+        <v>8</v>
+      </c>
+      <c r="B12" s="31">
+        <v>-44</v>
+      </c>
+      <c r="C12" s="31">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="D12" s="31">
+        <f t="shared" si="0"/>
+        <v>0.86999999999999988</v>
+      </c>
+      <c r="E12" s="31">
+        <v>1418.4</v>
+      </c>
+      <c r="F12" s="31">
+        <v>0.24507000000000001</v>
+      </c>
+      <c r="G12" s="31">
+        <v>150.43</v>
+      </c>
+      <c r="H12" s="31">
+        <v>386.23</v>
+      </c>
+      <c r="I12" s="31">
+        <v>0.80349999999999999</v>
+      </c>
+      <c r="J12" s="31">
+        <v>1.8326</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="33">
+        <v>9</v>
+      </c>
+      <c r="B13" s="31">
+        <v>-42</v>
+      </c>
+      <c r="C13" s="31">
+        <v>9.5750000000000002E-2</v>
+      </c>
+      <c r="D13" s="31">
+        <f t="shared" si="0"/>
+        <v>0.95750000000000002</v>
+      </c>
+      <c r="E13" s="31">
+        <v>1412.6</v>
+      </c>
+      <c r="F13" s="31">
+        <v>0.22409999999999999</v>
+      </c>
+      <c r="G13" s="31">
+        <v>152.61000000000001</v>
+      </c>
+      <c r="H13" s="31">
+        <v>387.17</v>
+      </c>
+      <c r="I13" s="31">
+        <v>0.81299999999999994</v>
+      </c>
+      <c r="J13" s="31">
+        <v>1.8277000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="33">
+        <v>10</v>
+      </c>
+      <c r="B14" s="31">
+        <v>-40</v>
+      </c>
+      <c r="C14" s="31">
+        <v>0.10131999999999999</v>
+      </c>
+      <c r="D14" s="31">
+        <f t="shared" si="0"/>
+        <v>1.0131999999999999</v>
+      </c>
+      <c r="E14" s="31">
+        <v>1409.1</v>
+      </c>
+      <c r="F14" s="31">
+        <v>0.21256</v>
+      </c>
+      <c r="G14" s="31">
+        <v>153.93</v>
+      </c>
+      <c r="H14" s="31">
+        <v>387.72</v>
+      </c>
+      <c r="I14" s="31">
+        <v>0.81859999999999999</v>
+      </c>
+      <c r="J14" s="31">
+        <v>1.8249</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="33">
+        <v>11</v>
+      </c>
+      <c r="B15" s="31">
+        <v>-40</v>
+      </c>
+      <c r="C15" s="31">
+        <v>0.10518</v>
+      </c>
+      <c r="D15" s="31">
+        <f t="shared" si="0"/>
+        <v>1.0518000000000001</v>
+      </c>
+      <c r="E15" s="31">
+        <v>1406.8</v>
+      </c>
+      <c r="F15" s="31">
+        <v>0.20526</v>
+      </c>
+      <c r="G15" s="31">
+        <v>154.80000000000001</v>
+      </c>
+      <c r="H15" s="31">
+        <v>388.09</v>
+      </c>
+      <c r="I15" s="31">
+        <v>0.82240000000000002</v>
+      </c>
+      <c r="J15" s="31">
+        <v>1.823</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="33">
+        <v>12</v>
+      </c>
+      <c r="B16" s="31">
+        <v>-38</v>
+      </c>
+      <c r="C16" s="31">
+        <v>0.11533</v>
+      </c>
+      <c r="D16" s="31">
+        <f t="shared" si="0"/>
+        <v>1.1533</v>
+      </c>
+      <c r="E16" s="31">
+        <v>1401</v>
+      </c>
+      <c r="F16" s="31">
+        <v>0.18831999999999999</v>
+      </c>
+      <c r="G16" s="31">
+        <v>156.99</v>
+      </c>
+      <c r="H16" s="31">
+        <v>389.01</v>
+      </c>
+      <c r="I16" s="31">
+        <v>0.83169999999999999</v>
+      </c>
+      <c r="J16" s="31">
+        <v>1.8184</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="33">
+        <v>13</v>
+      </c>
+      <c r="B17" s="31">
+        <v>-36</v>
+      </c>
+      <c r="C17" s="31">
+        <v>0.12623000000000001</v>
+      </c>
+      <c r="D17" s="31">
+        <f t="shared" si="0"/>
+        <v>1.2623000000000002</v>
+      </c>
+      <c r="E17" s="31">
+        <v>1395.1</v>
+      </c>
+      <c r="F17" s="31">
+        <v>0.17305999999999999</v>
+      </c>
+      <c r="G17" s="31">
+        <v>159.19</v>
+      </c>
+      <c r="H17" s="31">
+        <v>389.93</v>
+      </c>
+      <c r="I17" s="31">
+        <v>0.84099999999999997</v>
+      </c>
+      <c r="J17" s="31">
+        <v>1.8140000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="33">
+        <v>14</v>
+      </c>
+      <c r="B18" s="31">
+        <v>-34</v>
+      </c>
+      <c r="C18" s="31">
+        <v>0.13793</v>
+      </c>
+      <c r="D18" s="31">
+        <f t="shared" si="0"/>
+        <v>1.3793</v>
+      </c>
+      <c r="E18" s="31">
+        <v>1389.2</v>
+      </c>
+      <c r="F18" s="31">
+        <v>0.15926999999999999</v>
+      </c>
+      <c r="G18" s="31">
+        <v>161.4</v>
+      </c>
+      <c r="H18" s="31">
+        <v>390.84</v>
+      </c>
+      <c r="I18" s="31">
+        <v>0.85019999999999996</v>
+      </c>
+      <c r="J18" s="31">
+        <v>1.8096000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="33">
+        <v>15</v>
+      </c>
+      <c r="B19" s="31">
+        <v>-32</v>
+      </c>
+      <c r="C19" s="31">
+        <v>0.15045</v>
+      </c>
+      <c r="D19" s="31">
+        <f t="shared" si="0"/>
+        <v>1.5044999999999999</v>
+      </c>
+      <c r="E19" s="31">
+        <v>1383.3</v>
+      </c>
+      <c r="F19" s="31">
+        <v>0.14680000000000001</v>
+      </c>
+      <c r="G19" s="31">
+        <v>163.61000000000001</v>
+      </c>
+      <c r="H19" s="31">
+        <v>391.74</v>
+      </c>
+      <c r="I19" s="31">
+        <v>0.85940000000000005</v>
+      </c>
+      <c r="J19" s="31">
+        <v>1.8053999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="33">
+        <v>16</v>
+      </c>
+      <c r="B20" s="31">
+        <v>-30</v>
+      </c>
+      <c r="C20" s="31">
+        <v>0.16384000000000001</v>
+      </c>
+      <c r="D20" s="31">
+        <f t="shared" si="0"/>
+        <v>1.6384000000000001</v>
+      </c>
+      <c r="E20" s="31">
+        <v>1377.3</v>
+      </c>
+      <c r="F20" s="31">
+        <v>0.13550999999999999</v>
+      </c>
+      <c r="G20" s="31">
+        <v>165.82</v>
+      </c>
+      <c r="H20" s="31">
+        <v>392.63</v>
+      </c>
+      <c r="I20" s="31">
+        <v>0.86850000000000005</v>
+      </c>
+      <c r="J20" s="31">
+        <v>1.8012999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="33">
+        <v>17</v>
+      </c>
+      <c r="B21" s="31">
+        <v>-28</v>
+      </c>
+      <c r="C21" s="31">
+        <v>0.17815</v>
+      </c>
+      <c r="D21" s="31">
+        <f t="shared" si="0"/>
+        <v>1.7815000000000001</v>
+      </c>
+      <c r="E21" s="31">
+        <v>1371.3</v>
+      </c>
+      <c r="F21" s="31">
+        <v>0.12525</v>
+      </c>
+      <c r="G21" s="31">
+        <v>168.04</v>
+      </c>
+      <c r="H21" s="31">
+        <v>393.52</v>
+      </c>
+      <c r="I21" s="31">
+        <v>0.87760000000000005</v>
+      </c>
+      <c r="J21" s="31">
+        <v>1.7972999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="33">
+        <v>18</v>
+      </c>
+      <c r="B22" s="31">
+        <v>-26</v>
+      </c>
+      <c r="C22" s="31">
+        <v>0.19339999999999999</v>
+      </c>
+      <c r="D22" s="31">
+        <f t="shared" si="0"/>
+        <v>1.9339999999999999</v>
+      </c>
+      <c r="E22" s="31">
+        <v>1365.2</v>
+      </c>
+      <c r="F22" s="31">
+        <v>0.11593000000000001</v>
+      </c>
+      <c r="G22" s="31">
+        <v>170.27</v>
+      </c>
+      <c r="H22" s="31">
+        <v>394.39</v>
+      </c>
+      <c r="I22" s="31">
+        <v>0.88660000000000005</v>
+      </c>
+      <c r="J22" s="31">
+        <v>1.7934000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="33">
+        <v>19</v>
+      </c>
+      <c r="B23" s="31">
+        <v>-24</v>
+      </c>
+      <c r="C23" s="31">
+        <v>0.20965</v>
+      </c>
+      <c r="D23" s="31">
+        <f t="shared" si="0"/>
+        <v>2.0964999999999998</v>
+      </c>
+      <c r="E23" s="31">
+        <v>1359.1</v>
+      </c>
+      <c r="F23" s="31">
+        <v>0.10743999999999999</v>
+      </c>
+      <c r="G23" s="31">
+        <v>172.51</v>
+      </c>
+      <c r="H23" s="31">
+        <v>395.26</v>
+      </c>
+      <c r="I23" s="31">
+        <v>0.89549999999999996</v>
+      </c>
+      <c r="J23" s="31">
+        <v>1.7896000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="33">
+        <v>20</v>
+      </c>
+      <c r="B24" s="31">
+        <v>-22</v>
+      </c>
+      <c r="C24" s="31">
+        <v>0.22692999999999999</v>
+      </c>
+      <c r="D24" s="31">
+        <f t="shared" si="0"/>
+        <v>2.2692999999999999</v>
+      </c>
+      <c r="E24" s="31">
+        <v>1352.9</v>
+      </c>
+      <c r="F24" s="31">
+        <v>9.9699999999999997E-2</v>
+      </c>
+      <c r="G24" s="31">
+        <v>174.75</v>
+      </c>
+      <c r="H24" s="31">
+        <v>396.12</v>
+      </c>
+      <c r="I24" s="31">
+        <v>0.90439999999999998</v>
+      </c>
+      <c r="J24" s="31">
+        <v>1.7859</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="33">
+        <v>21</v>
+      </c>
+      <c r="B25" s="31">
+        <v>-20</v>
+      </c>
+      <c r="C25" s="31">
+        <v>0.24529000000000001</v>
+      </c>
+      <c r="D25" s="31">
+        <f t="shared" si="0"/>
+        <v>2.4529000000000001</v>
+      </c>
+      <c r="E25" s="31">
+        <v>1346.8</v>
+      </c>
+      <c r="F25" s="31">
+        <v>9.2619999999999994E-2</v>
+      </c>
+      <c r="G25" s="31">
+        <v>177</v>
+      </c>
+      <c r="H25" s="31">
+        <v>396.67</v>
+      </c>
+      <c r="I25" s="31">
+        <v>0.9133</v>
+      </c>
+      <c r="J25" s="31">
+        <v>1.7822</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="33">
+        <v>22</v>
+      </c>
+      <c r="B26" s="31">
+        <v>-18</v>
+      </c>
+      <c r="C26" s="31">
+        <v>0.26477000000000001</v>
+      </c>
+      <c r="D26" s="31">
+        <f t="shared" si="0"/>
+        <v>2.6476999999999999</v>
+      </c>
+      <c r="E26" s="31">
+        <v>1340.5</v>
+      </c>
+      <c r="F26" s="31">
+        <v>8.6150000000000004E-2</v>
+      </c>
+      <c r="G26" s="31">
+        <v>179.26</v>
+      </c>
+      <c r="H26" s="31">
+        <v>397.81</v>
+      </c>
+      <c r="I26" s="31">
+        <v>0.92220000000000002</v>
+      </c>
+      <c r="J26" s="31">
+        <v>1.7786999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="33">
+        <v>23</v>
+      </c>
+      <c r="B27" s="31">
+        <v>-16</v>
+      </c>
+      <c r="C27" s="31">
+        <v>0.28542000000000001</v>
+      </c>
+      <c r="D27" s="31">
+        <f t="shared" si="0"/>
+        <v>2.8542000000000001</v>
+      </c>
+      <c r="E27" s="31">
+        <v>1334.2</v>
+      </c>
+      <c r="F27" s="31">
+        <v>8.0229999999999996E-2</v>
+      </c>
+      <c r="G27" s="31">
+        <v>181.53</v>
+      </c>
+      <c r="H27" s="31">
+        <v>398.64</v>
+      </c>
+      <c r="I27" s="31">
+        <v>0.93089999999999995</v>
+      </c>
+      <c r="J27" s="31">
+        <v>1.7751999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="33">
+        <v>24</v>
+      </c>
+      <c r="B28" s="31">
+        <v>-14</v>
+      </c>
+      <c r="C28" s="31">
+        <v>0.30728</v>
+      </c>
+      <c r="D28" s="31">
+        <f t="shared" si="0"/>
+        <v>3.0728</v>
+      </c>
+      <c r="E28" s="31">
+        <v>1327.9</v>
+      </c>
+      <c r="F28" s="31">
+        <v>7.4789999999999995E-2</v>
+      </c>
+      <c r="G28" s="31">
+        <v>183.81</v>
+      </c>
+      <c r="H28" s="31">
+        <v>399.46</v>
+      </c>
+      <c r="I28" s="31">
+        <v>0.93969999999999998</v>
+      </c>
+      <c r="J28" s="31">
+        <v>1.7719</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="33">
+        <v>25</v>
+      </c>
+      <c r="B29" s="31">
+        <v>-12</v>
+      </c>
+      <c r="C29" s="31">
+        <v>0.33040000000000003</v>
+      </c>
+      <c r="D29" s="31">
+        <f t="shared" si="0"/>
+        <v>3.3040000000000003</v>
+      </c>
+      <c r="E29" s="31">
+        <v>1321.5</v>
+      </c>
+      <c r="F29" s="31">
+        <v>6.9790000000000005E-2</v>
+      </c>
+      <c r="G29" s="31">
+        <v>186.09</v>
+      </c>
+      <c r="H29" s="31">
+        <v>400.27</v>
+      </c>
+      <c r="I29" s="31">
+        <v>0.94840000000000002</v>
+      </c>
+      <c r="J29" s="31">
+        <v>1.7685999999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="33">
+        <v>26</v>
+      </c>
+      <c r="B30" s="31">
+        <v>-10</v>
+      </c>
+      <c r="C30" s="31">
+        <v>0.35482000000000002</v>
+      </c>
+      <c r="D30" s="31">
+        <f t="shared" si="0"/>
+        <v>3.5482000000000005</v>
+      </c>
+      <c r="E30" s="31">
+        <v>1315</v>
+      </c>
+      <c r="F30" s="31">
+        <v>6.5199999999999994E-2</v>
+      </c>
+      <c r="G30" s="31">
+        <v>188.38</v>
+      </c>
+      <c r="H30" s="31">
+        <v>401.07</v>
+      </c>
+      <c r="I30" s="31">
+        <v>0.95709999999999995</v>
+      </c>
+      <c r="J30" s="31">
+        <v>1.7653000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="33">
+        <v>27</v>
+      </c>
+      <c r="B31" s="31">
+        <v>-8</v>
+      </c>
+      <c r="C31" s="31">
+        <v>0.38058999999999998</v>
+      </c>
+      <c r="D31" s="31">
+        <f t="shared" si="0"/>
+        <v>3.8058999999999998</v>
+      </c>
+      <c r="E31" s="31">
+        <v>1308.5</v>
+      </c>
+      <c r="F31" s="31">
+        <v>6.096E-2</v>
+      </c>
+      <c r="G31" s="31">
+        <v>190.69</v>
+      </c>
+      <c r="H31" s="31">
+        <v>401.85</v>
+      </c>
+      <c r="I31" s="31">
+        <v>0.9657</v>
+      </c>
+      <c r="J31" s="31">
+        <v>1.7621</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="33">
+        <v>28</v>
+      </c>
+      <c r="B32" s="31">
+        <v>-6</v>
+      </c>
+      <c r="C32" s="31">
+        <v>0.40775</v>
+      </c>
+      <c r="D32" s="31">
+        <f t="shared" si="0"/>
+        <v>4.0774999999999997</v>
+      </c>
+      <c r="E32" s="31">
+        <v>1301.9000000000001</v>
+      </c>
+      <c r="F32" s="31">
+        <v>5.706E-2</v>
+      </c>
+      <c r="G32" s="31">
+        <v>193</v>
+      </c>
+      <c r="H32" s="31">
+        <v>402.63</v>
+      </c>
+      <c r="I32" s="31">
+        <v>0.97430000000000005</v>
+      </c>
+      <c r="J32" s="31">
+        <v>1.7589999999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="33">
+        <v>29</v>
+      </c>
+      <c r="B33" s="31">
+        <v>-4</v>
+      </c>
+      <c r="C33" s="31">
+        <v>0.43636000000000003</v>
+      </c>
+      <c r="D33" s="31">
+        <f t="shared" si="0"/>
+        <v>4.3635999999999999</v>
+      </c>
+      <c r="E33" s="31">
+        <v>1295.3</v>
+      </c>
+      <c r="F33" s="31">
+        <v>5.3449999999999998E-2</v>
+      </c>
+      <c r="G33" s="31">
+        <v>195.32</v>
+      </c>
+      <c r="H33" s="31">
+        <v>403.39</v>
+      </c>
+      <c r="I33" s="31">
+        <v>0.9829</v>
+      </c>
+      <c r="J33" s="31">
+        <v>1.756</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="33">
+        <v>30</v>
+      </c>
+      <c r="B34" s="31">
+        <v>-2</v>
+      </c>
+      <c r="C34" s="31">
+        <v>0.46645999999999999</v>
+      </c>
+      <c r="D34" s="31">
+        <f t="shared" si="0"/>
+        <v>4.6646000000000001</v>
+      </c>
+      <c r="E34" s="31">
+        <v>1288.5999999999999</v>
+      </c>
+      <c r="F34" s="31">
+        <v>5.0119999999999998E-2</v>
+      </c>
+      <c r="G34" s="31">
+        <v>197.66</v>
+      </c>
+      <c r="H34" s="31">
+        <v>404.14</v>
+      </c>
+      <c r="I34" s="31">
+        <v>0.99150000000000005</v>
+      </c>
+      <c r="J34" s="31">
+        <v>1.7529999999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="33">
+        <v>31</v>
+      </c>
+      <c r="B35" s="42">
+        <v>0</v>
+      </c>
+      <c r="C35" s="42">
+        <v>0.49811</v>
+      </c>
+      <c r="D35" s="42">
+        <f t="shared" si="0"/>
+        <v>4.9810999999999996</v>
+      </c>
+      <c r="E35" s="42">
+        <v>1281.8</v>
+      </c>
+      <c r="F35" s="42">
+        <v>4.7030000000000002E-2</v>
+      </c>
+      <c r="G35" s="42">
+        <v>200</v>
+      </c>
+      <c r="H35" s="42">
+        <v>404.87</v>
+      </c>
+      <c r="I35" s="42">
+        <v>1</v>
+      </c>
+      <c r="J35" s="42">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B36" s="31">
+        <v>2</v>
+      </c>
+      <c r="C36" s="31">
+        <v>0.53134000000000003</v>
+      </c>
+      <c r="D36" s="31">
+        <f t="shared" ref="D36:D67" si="1">C36*10</f>
+        <v>5.3134000000000006</v>
+      </c>
+      <c r="E36" s="31">
+        <v>1275</v>
+      </c>
+      <c r="F36" s="31">
+        <v>4.4170000000000001E-2</v>
+      </c>
+      <c r="G36" s="31">
+        <v>202.35</v>
+      </c>
+      <c r="H36" s="31">
+        <v>405.59</v>
+      </c>
+      <c r="I36" s="31">
+        <v>1.0085</v>
+      </c>
+      <c r="J36" s="31">
+        <v>1.7471000000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B37" s="31">
+        <v>4</v>
+      </c>
+      <c r="C37" s="31">
+        <v>0.56621999999999995</v>
+      </c>
+      <c r="D37" s="31">
+        <f t="shared" si="1"/>
+        <v>5.6621999999999995</v>
+      </c>
+      <c r="E37" s="31">
+        <v>1268.0999999999999</v>
+      </c>
+      <c r="F37" s="31">
+        <v>4.1520000000000001E-2</v>
+      </c>
+      <c r="G37" s="31">
+        <v>204.72</v>
+      </c>
+      <c r="H37" s="31">
+        <v>406.3</v>
+      </c>
+      <c r="I37" s="31">
+        <v>1.0169999999999999</v>
+      </c>
+      <c r="J37" s="31">
+        <v>1.7443</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B38" s="31">
+        <v>6</v>
+      </c>
+      <c r="C38" s="31">
+        <v>0.60279000000000005</v>
+      </c>
+      <c r="D38" s="31">
+        <f t="shared" si="1"/>
+        <v>6.0279000000000007</v>
+      </c>
+      <c r="E38" s="31">
+        <v>1261.0999999999999</v>
+      </c>
+      <c r="F38" s="31">
+        <v>3.9059999999999997E-2</v>
+      </c>
+      <c r="G38" s="31">
+        <v>207.1</v>
+      </c>
+      <c r="H38" s="31">
+        <v>406.99</v>
+      </c>
+      <c r="I38" s="31">
+        <v>1.0254000000000001</v>
+      </c>
+      <c r="J38" s="31">
+        <v>1.7415</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B39" s="31">
+        <v>8</v>
+      </c>
+      <c r="C39" s="31">
+        <v>0.64109000000000005</v>
+      </c>
+      <c r="D39" s="31">
+        <f t="shared" si="1"/>
+        <v>6.4109000000000007</v>
+      </c>
+      <c r="E39" s="31">
+        <v>1254</v>
+      </c>
+      <c r="F39" s="31">
+        <v>3.6760000000000001E-2</v>
+      </c>
+      <c r="G39" s="31">
+        <v>209.49</v>
+      </c>
+      <c r="H39" s="31">
+        <v>407.67</v>
+      </c>
+      <c r="I39" s="31">
+        <v>1.0338000000000001</v>
+      </c>
+      <c r="J39" s="31">
+        <v>1.7386999999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B40" s="31">
+        <v>10</v>
+      </c>
+      <c r="C40" s="31">
+        <v>0.68118999999999996</v>
+      </c>
+      <c r="D40" s="31">
+        <f t="shared" si="1"/>
+        <v>6.8118999999999996</v>
+      </c>
+      <c r="E40" s="31">
+        <v>1246.9000000000001</v>
+      </c>
+      <c r="F40" s="31">
+        <v>3.4630000000000001E-2</v>
+      </c>
+      <c r="G40" s="31">
+        <v>211.89</v>
+      </c>
+      <c r="H40" s="31">
+        <v>408.33</v>
+      </c>
+      <c r="I40" s="31">
+        <v>1.0422</v>
+      </c>
+      <c r="J40" s="31">
+        <v>1.736</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B41" s="31">
+        <v>12</v>
+      </c>
+      <c r="C41" s="31">
+        <v>0.72314000000000001</v>
+      </c>
+      <c r="D41" s="31">
+        <f t="shared" si="1"/>
+        <v>7.2313999999999998</v>
+      </c>
+      <c r="E41" s="31">
+        <v>1239.7</v>
+      </c>
+      <c r="F41" s="31">
+        <v>3.2649999999999998E-2</v>
+      </c>
+      <c r="G41" s="31">
+        <v>214.31</v>
+      </c>
+      <c r="H41" s="31">
+        <v>408.97</v>
+      </c>
+      <c r="I41" s="31">
+        <v>1.0506</v>
+      </c>
+      <c r="J41" s="31">
+        <v>1.7333000000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B42" s="31">
+        <v>14</v>
+      </c>
+      <c r="C42" s="31">
+        <v>0.76698</v>
+      </c>
+      <c r="D42" s="31">
+        <f t="shared" si="1"/>
+        <v>7.6698000000000004</v>
+      </c>
+      <c r="E42" s="31">
+        <v>1232.4000000000001</v>
+      </c>
+      <c r="F42" s="31">
+        <v>3.0790000000000001E-2</v>
+      </c>
+      <c r="G42" s="31">
+        <v>216.74</v>
+      </c>
+      <c r="H42" s="31">
+        <v>409.6</v>
+      </c>
+      <c r="I42" s="31">
+        <v>1.0589999999999999</v>
+      </c>
+      <c r="J42" s="31">
+        <v>1.7305999999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B43" s="31">
+        <v>16</v>
+      </c>
+      <c r="C43" s="31">
+        <v>0.81276999999999999</v>
+      </c>
+      <c r="D43" s="31">
+        <f t="shared" si="1"/>
+        <v>8.1277000000000008</v>
+      </c>
+      <c r="E43" s="31">
+        <v>1225</v>
+      </c>
+      <c r="F43" s="31">
+        <v>2.9059999999999999E-2</v>
+      </c>
+      <c r="G43" s="31">
+        <v>219.18</v>
+      </c>
+      <c r="H43" s="31">
+        <v>410.21</v>
+      </c>
+      <c r="I43" s="31">
+        <v>1.0672999999999999</v>
+      </c>
+      <c r="J43" s="31">
+        <v>1.728</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B44" s="31">
+        <v>18</v>
+      </c>
+      <c r="C44" s="31">
+        <v>0.86055999999999999</v>
+      </c>
+      <c r="D44" s="31">
+        <f t="shared" si="1"/>
+        <v>8.605599999999999</v>
+      </c>
+      <c r="E44" s="31">
+        <v>1217.5999999999999</v>
+      </c>
+      <c r="F44" s="31">
+        <v>2.7439999999999999E-2</v>
+      </c>
+      <c r="G44" s="31">
+        <v>221.63</v>
+      </c>
+      <c r="H44" s="31">
+        <v>410.8</v>
+      </c>
+      <c r="I44" s="31">
+        <v>1.0755999999999999</v>
+      </c>
+      <c r="J44" s="31">
+        <v>1.7254</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B45" s="31">
+        <v>20</v>
+      </c>
+      <c r="C45" s="31">
+        <v>0.91041000000000005</v>
+      </c>
+      <c r="D45" s="31">
+        <f t="shared" si="1"/>
+        <v>9.1041000000000007</v>
+      </c>
+      <c r="E45" s="31">
+        <v>1210</v>
+      </c>
+      <c r="F45" s="31">
+        <v>2.5930000000000002E-2</v>
+      </c>
+      <c r="G45" s="31">
+        <v>224.1</v>
+      </c>
+      <c r="H45" s="31">
+        <v>411.38</v>
+      </c>
+      <c r="I45" s="31">
+        <v>1.0840000000000001</v>
+      </c>
+      <c r="J45" s="31">
+        <v>1.7228000000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B46" s="31">
+        <v>22</v>
+      </c>
+      <c r="C46" s="31">
+        <v>0.96235999999999999</v>
+      </c>
+      <c r="D46" s="31">
+        <f t="shared" si="1"/>
+        <v>9.6235999999999997</v>
+      </c>
+      <c r="E46" s="31">
+        <v>1202.4000000000001</v>
+      </c>
+      <c r="F46" s="31">
+        <v>2.4510000000000001E-2</v>
+      </c>
+      <c r="G46" s="31">
+        <v>226.59</v>
+      </c>
+      <c r="H46" s="31">
+        <v>411.93</v>
+      </c>
+      <c r="I46" s="31">
+        <v>1.0923</v>
+      </c>
+      <c r="J46" s="31">
+        <v>1.7202</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B47" s="31">
+        <v>24</v>
+      </c>
+      <c r="C47" s="31">
+        <v>1.0165</v>
+      </c>
+      <c r="D47" s="31">
+        <f t="shared" si="1"/>
+        <v>10.164999999999999</v>
+      </c>
+      <c r="E47" s="31">
+        <v>1194.5999999999999</v>
+      </c>
+      <c r="F47" s="31">
+        <v>2.3189999999999999E-2</v>
+      </c>
+      <c r="G47" s="31">
+        <v>229.09</v>
+      </c>
+      <c r="H47" s="31">
+        <v>412.46</v>
+      </c>
+      <c r="I47" s="31">
+        <v>1.1006</v>
+      </c>
+      <c r="J47" s="31">
+        <v>1.7177</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B48" s="31">
+        <v>26</v>
+      </c>
+      <c r="C48" s="31">
+        <v>1.0728</v>
+      </c>
+      <c r="D48" s="31">
+        <f t="shared" si="1"/>
+        <v>10.728</v>
+      </c>
+      <c r="E48" s="31">
+        <v>1186.8</v>
+      </c>
+      <c r="F48" s="31">
+        <v>2.1940000000000001E-2</v>
+      </c>
+      <c r="G48" s="31">
+        <v>231.6</v>
+      </c>
+      <c r="H48" s="31">
+        <v>412.98</v>
+      </c>
+      <c r="I48" s="31">
+        <v>1.1088</v>
+      </c>
+      <c r="J48" s="31">
+        <v>1.7151000000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B49" s="31">
+        <v>28</v>
+      </c>
+      <c r="C49" s="31">
+        <v>1.1314</v>
+      </c>
+      <c r="D49" s="31">
+        <f t="shared" si="1"/>
+        <v>11.314</v>
+      </c>
+      <c r="E49" s="31">
+        <v>1178.8</v>
+      </c>
+      <c r="F49" s="31">
+        <v>2.077E-2</v>
+      </c>
+      <c r="G49" s="31">
+        <v>234.14</v>
+      </c>
+      <c r="H49" s="31">
+        <v>413.46</v>
+      </c>
+      <c r="I49" s="31">
+        <v>1.1171</v>
+      </c>
+      <c r="J49" s="31">
+        <v>1.7125999999999999</v>
+      </c>
+    </row>
+    <row r="50" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B50" s="31">
+        <v>30</v>
+      </c>
+      <c r="C50" s="31">
+        <v>1.1923999999999999</v>
+      </c>
+      <c r="D50" s="31">
+        <f t="shared" si="1"/>
+        <v>11.923999999999999</v>
+      </c>
+      <c r="E50" s="31">
+        <v>1170.7</v>
+      </c>
+      <c r="F50" s="31">
+        <v>1.968E-2</v>
+      </c>
+      <c r="G50" s="31">
+        <v>236.69</v>
+      </c>
+      <c r="H50" s="31">
+        <v>413.93</v>
+      </c>
+      <c r="I50" s="31">
+        <v>1.1254</v>
+      </c>
+      <c r="J50" s="31">
+        <v>1.7101</v>
+      </c>
+    </row>
+    <row r="51" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B51" s="31">
+        <v>32</v>
+      </c>
+      <c r="C51" s="31">
+        <v>1.2557</v>
+      </c>
+      <c r="D51" s="31">
+        <f t="shared" si="1"/>
+        <v>12.557</v>
+      </c>
+      <c r="E51" s="31">
+        <v>1162.5</v>
+      </c>
+      <c r="F51" s="31">
+        <v>1.864E-2</v>
+      </c>
+      <c r="G51" s="31">
+        <v>239.25</v>
+      </c>
+      <c r="H51" s="31">
+        <v>414.37</v>
+      </c>
+      <c r="I51" s="31">
+        <v>1.1335999999999999</v>
+      </c>
+      <c r="J51" s="31">
+        <v>1.7075</v>
+      </c>
+    </row>
+    <row r="52" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B52" s="31">
+        <v>34</v>
+      </c>
+      <c r="C52" s="31">
+        <v>1.3214999999999999</v>
+      </c>
+      <c r="D52" s="31">
+        <f t="shared" si="1"/>
+        <v>13.215</v>
+      </c>
+      <c r="E52" s="31">
+        <v>1154.2</v>
+      </c>
+      <c r="F52" s="31">
+        <v>1.7670000000000002E-2</v>
+      </c>
+      <c r="G52" s="31">
+        <v>241.84</v>
+      </c>
+      <c r="H52" s="31">
+        <v>414.79</v>
+      </c>
+      <c r="I52" s="31">
+        <v>1.1418999999999999</v>
+      </c>
+      <c r="J52" s="31">
+        <v>1.7050000000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B53" s="31">
+        <v>36</v>
+      </c>
+      <c r="C53" s="31">
+        <v>1.3897999999999999</v>
+      </c>
+      <c r="D53" s="31">
+        <f t="shared" si="1"/>
+        <v>13.898</v>
+      </c>
+      <c r="E53" s="31">
+        <v>1145.7</v>
+      </c>
+      <c r="F53" s="31">
+        <v>1.6750000000000001E-2</v>
+      </c>
+      <c r="G53" s="31">
+        <v>244.44</v>
+      </c>
+      <c r="H53" s="31">
+        <v>415.18</v>
+      </c>
+      <c r="I53" s="31">
+        <v>1.1500999999999999</v>
+      </c>
+      <c r="J53" s="31">
+        <v>1.7023999999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B54" s="31">
+        <v>38</v>
+      </c>
+      <c r="C54" s="31">
+        <v>1.4605999999999999</v>
+      </c>
+      <c r="D54" s="31">
+        <f t="shared" si="1"/>
+        <v>14.605999999999998</v>
+      </c>
+      <c r="E54" s="31">
+        <v>1137.0999999999999</v>
+      </c>
+      <c r="F54" s="31">
+        <v>1.5890000000000001E-2</v>
+      </c>
+      <c r="G54" s="31">
+        <v>247.06</v>
+      </c>
+      <c r="H54" s="31">
+        <v>415.54</v>
+      </c>
+      <c r="I54" s="31">
+        <v>1.1584000000000001</v>
+      </c>
+      <c r="J54" s="31">
+        <v>1.6999</v>
+      </c>
+    </row>
+    <row r="55" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B55" s="31">
+        <v>40</v>
+      </c>
+      <c r="C55" s="31">
+        <v>1.5341</v>
+      </c>
+      <c r="D55" s="31">
+        <f t="shared" si="1"/>
+        <v>15.341000000000001</v>
+      </c>
+      <c r="E55" s="31">
+        <v>1128.4000000000001</v>
+      </c>
+      <c r="F55" s="31">
+        <v>1.507E-2</v>
+      </c>
+      <c r="G55" s="31">
+        <v>249.71</v>
+      </c>
+      <c r="H55" s="31">
+        <v>415.87</v>
+      </c>
+      <c r="I55" s="31">
+        <v>1.1667000000000001</v>
+      </c>
+      <c r="J55" s="31">
+        <v>1.6973</v>
+      </c>
+    </row>
+    <row r="56" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B56" s="31">
+        <v>42</v>
+      </c>
+      <c r="C56" s="31">
+        <v>1.6103000000000001</v>
+      </c>
+      <c r="D56" s="31">
+        <f t="shared" si="1"/>
+        <v>16.103000000000002</v>
+      </c>
+      <c r="E56" s="31">
+        <v>1119.5</v>
+      </c>
+      <c r="F56" s="31">
+        <v>1.43E-2</v>
+      </c>
+      <c r="G56" s="31">
+        <v>252.37</v>
+      </c>
+      <c r="H56" s="31">
+        <v>416.17</v>
+      </c>
+      <c r="I56" s="31">
+        <v>1.1749000000000001</v>
+      </c>
+      <c r="J56" s="31">
+        <v>1.6947000000000001</v>
+      </c>
+    </row>
+    <row r="57" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B57" s="31">
+        <v>44</v>
+      </c>
+      <c r="C57" s="31">
+        <v>1.6892</v>
+      </c>
+      <c r="D57" s="31">
+        <f t="shared" si="1"/>
+        <v>16.891999999999999</v>
+      </c>
+      <c r="E57" s="31">
+        <v>1110.4000000000001</v>
+      </c>
+      <c r="F57" s="31">
+        <v>1.357E-2</v>
+      </c>
+      <c r="G57" s="31">
+        <v>255.06</v>
+      </c>
+      <c r="H57" s="31">
+        <v>416.44</v>
+      </c>
+      <c r="I57" s="31">
+        <v>1.1832</v>
+      </c>
+      <c r="J57" s="31">
+        <v>1.6920999999999999</v>
+      </c>
+    </row>
+    <row r="58" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B58" s="31">
+        <v>46</v>
+      </c>
+      <c r="C58" s="31">
+        <v>1.7708999999999999</v>
+      </c>
+      <c r="D58" s="31">
+        <f t="shared" si="1"/>
+        <v>17.709</v>
+      </c>
+      <c r="E58" s="31">
+        <v>1101.2</v>
+      </c>
+      <c r="F58" s="31">
+        <v>1.2880000000000001E-2</v>
+      </c>
+      <c r="G58" s="31">
+        <v>257.77</v>
+      </c>
+      <c r="H58" s="31">
+        <v>416.68</v>
+      </c>
+      <c r="I58" s="31">
+        <v>1.1915</v>
+      </c>
+      <c r="J58" s="31">
+        <v>1.6894</v>
+      </c>
+    </row>
+    <row r="59" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B59" s="31">
+        <v>48</v>
+      </c>
+      <c r="C59" s="31">
+        <v>1.8554999999999999</v>
+      </c>
+      <c r="D59" s="31">
+        <f t="shared" si="1"/>
+        <v>18.555</v>
+      </c>
+      <c r="E59" s="31">
+        <v>1091.8</v>
+      </c>
+      <c r="F59" s="31">
+        <v>1.223E-2</v>
+      </c>
+      <c r="G59" s="31">
+        <v>260.51</v>
+      </c>
+      <c r="H59" s="31">
+        <v>416.87</v>
+      </c>
+      <c r="I59" s="31">
+        <v>1.1998</v>
+      </c>
+      <c r="J59" s="31">
+        <v>1.6867000000000001</v>
+      </c>
+    </row>
+    <row r="60" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B60" s="31">
+        <v>50</v>
+      </c>
+      <c r="C60" s="31">
+        <v>1.9431</v>
+      </c>
+      <c r="D60" s="31">
+        <f t="shared" si="1"/>
+        <v>19.431000000000001</v>
+      </c>
+      <c r="E60" s="31">
+        <v>1082.0999999999999</v>
+      </c>
+      <c r="F60" s="31">
+        <v>1.1610000000000001E-2</v>
+      </c>
+      <c r="G60" s="31">
+        <v>263.27</v>
+      </c>
+      <c r="H60" s="31">
+        <v>417.03</v>
+      </c>
+      <c r="I60" s="31">
+        <v>1.2081</v>
+      </c>
+      <c r="J60" s="31">
+        <v>1.6839999999999999</v>
+      </c>
+    </row>
+    <row r="61" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B61" s="31">
+        <v>55</v>
+      </c>
+      <c r="C61" s="31">
+        <v>2.1753</v>
+      </c>
+      <c r="D61" s="31">
+        <f t="shared" si="1"/>
+        <v>21.753</v>
+      </c>
+      <c r="E61" s="31">
+        <v>1057.0999999999999</v>
+      </c>
+      <c r="F61" s="31">
+        <v>1.0200000000000001E-2</v>
+      </c>
+      <c r="G61" s="31">
+        <v>270.31</v>
+      </c>
+      <c r="H61" s="31">
+        <v>417.24</v>
+      </c>
+      <c r="I61" s="31">
+        <v>1.2291000000000001</v>
+      </c>
+      <c r="J61" s="31">
+        <v>1.6768000000000001</v>
+      </c>
+    </row>
+    <row r="62" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B62" s="31">
+        <v>60</v>
+      </c>
+      <c r="C62" s="31">
+        <v>2.4274</v>
+      </c>
+      <c r="D62" s="31">
+        <f t="shared" si="1"/>
+        <v>24.274000000000001</v>
+      </c>
+      <c r="E62" s="31">
+        <v>1030.5</v>
+      </c>
+      <c r="F62" s="31">
+        <v>8.9499999999999996E-3</v>
+      </c>
+      <c r="G62" s="31">
+        <v>277.56</v>
+      </c>
+      <c r="H62" s="31">
+        <v>417.14</v>
+      </c>
+      <c r="I62" s="31">
+        <v>1.2503</v>
+      </c>
+      <c r="J62" s="31">
+        <v>1.6692</v>
+      </c>
+    </row>
+    <row r="63" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B63" s="31">
+        <v>65</v>
+      </c>
+      <c r="C63" s="31">
+        <v>2.7008000000000001</v>
+      </c>
+      <c r="D63" s="31">
+        <f t="shared" si="1"/>
+        <v>27.008000000000003</v>
+      </c>
+      <c r="E63" s="31">
+        <v>1001.8</v>
+      </c>
+      <c r="F63" s="31">
+        <v>7.8399999999999997E-3</v>
+      </c>
+      <c r="G63" s="31">
+        <v>285.06</v>
+      </c>
+      <c r="H63" s="31">
+        <v>416.65</v>
+      </c>
+      <c r="I63" s="31">
+        <v>1.2718</v>
+      </c>
+      <c r="J63" s="31">
+        <v>1.661</v>
+      </c>
+    </row>
+    <row r="64" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B64" s="31">
+        <v>70</v>
+      </c>
+      <c r="C64" s="31">
+        <v>2.9967000000000001</v>
+      </c>
+      <c r="D64" s="31">
+        <f t="shared" si="1"/>
+        <v>29.967000000000002</v>
+      </c>
+      <c r="E64" s="31">
+        <v>970.4</v>
+      </c>
+      <c r="F64" s="31">
+        <v>6.8399999999999997E-3</v>
+      </c>
+      <c r="G64" s="31">
+        <v>292.89999999999998</v>
+      </c>
+      <c r="H64" s="31">
+        <v>415.69</v>
+      </c>
+      <c r="I64" s="31">
+        <v>1.294</v>
+      </c>
+      <c r="J64" s="31">
+        <v>1.6517999999999999</v>
+      </c>
+    </row>
+    <row r="65" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B65" s="31">
+        <v>75</v>
+      </c>
+      <c r="C65" s="31">
+        <v>3.3168000000000002</v>
+      </c>
+      <c r="D65" s="31">
+        <f t="shared" si="1"/>
+        <v>33.167999999999999</v>
+      </c>
+      <c r="E65" s="31">
+        <v>935.3</v>
+      </c>
+      <c r="F65" s="31">
+        <v>5.94E-3</v>
+      </c>
+      <c r="G65" s="31">
+        <v>301.18</v>
+      </c>
+      <c r="H65" s="31">
+        <v>414.09</v>
+      </c>
+      <c r="I65" s="31">
+        <v>1.3169</v>
+      </c>
+      <c r="J65" s="31">
+        <v>1.6413</v>
+      </c>
+    </row>
+    <row r="66" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B66" s="31">
+        <v>80</v>
+      </c>
+      <c r="C66" s="31">
+        <v>3.6627000000000001</v>
+      </c>
+      <c r="D66" s="31">
+        <f t="shared" si="1"/>
+        <v>36.627000000000002</v>
+      </c>
+      <c r="E66" s="31">
+        <v>894.8</v>
+      </c>
+      <c r="F66" s="31">
+        <v>5.11E-3</v>
+      </c>
+      <c r="G66" s="31">
+        <v>310.10000000000002</v>
+      </c>
+      <c r="H66" s="31">
+        <v>411.6</v>
+      </c>
+      <c r="I66" s="31">
+        <v>1.3412999999999999</v>
+      </c>
+      <c r="J66" s="31">
+        <v>1.6287</v>
+      </c>
+    </row>
+    <row r="67" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B67" s="31">
+        <v>85</v>
+      </c>
+      <c r="C67" s="31">
+        <v>4.0368000000000004</v>
+      </c>
+      <c r="D67" s="31">
+        <f t="shared" si="1"/>
+        <v>40.368000000000002</v>
+      </c>
+      <c r="E67" s="31">
+        <v>845.1</v>
+      </c>
+      <c r="F67" s="31">
+        <v>4.3299999999999996E-3</v>
+      </c>
+      <c r="G67" s="31">
+        <v>320.05</v>
+      </c>
+      <c r="H67" s="31">
+        <v>407.72</v>
+      </c>
+      <c r="I67" s="31">
+        <v>1.3680000000000001</v>
+      </c>
+      <c r="J67" s="31">
+        <v>1.6128</v>
+      </c>
+    </row>
+    <row r="68" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B68" s="31">
+        <v>90</v>
+      </c>
+      <c r="C68" s="31">
+        <v>4.4416000000000002</v>
+      </c>
+      <c r="D68" s="31">
+        <f t="shared" ref="D68:D70" si="2">C68*10</f>
+        <v>44.416000000000004</v>
+      </c>
+      <c r="E68" s="31">
+        <v>777.5</v>
+      </c>
+      <c r="F68" s="31">
+        <v>3.5500000000000002E-3</v>
+      </c>
+      <c r="G68" s="31">
+        <v>331.98</v>
+      </c>
+      <c r="H68" s="31">
+        <v>401.33</v>
+      </c>
+      <c r="I68" s="31">
+        <v>1.3997999999999999</v>
+      </c>
+      <c r="J68" s="31">
+        <v>1.5907</v>
+      </c>
+    </row>
+    <row r="69" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B69" s="31">
+        <v>95</v>
+      </c>
+      <c r="C69" s="31">
+        <v>4.8819999999999997</v>
+      </c>
+      <c r="D69" s="31">
+        <f t="shared" si="2"/>
+        <v>48.819999999999993</v>
+      </c>
+      <c r="E69" s="31">
+        <v>665.4</v>
+      </c>
+      <c r="F69" s="31">
+        <v>2.64E-3</v>
+      </c>
+      <c r="G69" s="31">
+        <v>348.86</v>
+      </c>
+      <c r="H69" s="31">
+        <v>387.46</v>
+      </c>
+      <c r="I69" s="31">
+        <v>1.4441999999999999</v>
+      </c>
+      <c r="J69" s="31">
+        <v>1.5490999999999999</v>
+      </c>
+    </row>
+    <row r="70" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B70" s="31">
+        <v>96.14</v>
+      </c>
+      <c r="C70" s="31">
+        <v>4.99</v>
+      </c>
+      <c r="D70" s="31">
+        <f t="shared" si="2"/>
+        <v>49.900000000000006</v>
+      </c>
+      <c r="E70" s="31">
+        <v>523.79999999999995</v>
+      </c>
+      <c r="F70" s="31">
+        <v>1.91E-3</v>
+      </c>
+      <c r="G70" s="31">
+        <v>366.59</v>
+      </c>
+      <c r="H70" s="31">
+        <v>366.59</v>
+      </c>
+      <c r="I70" s="31">
+        <v>1.4918</v>
+      </c>
+      <c r="J70" s="31">
+        <v>1.4918</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D69"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="2:4" ht="48" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="46" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="46" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" ht="16.5" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="36">
+        <v>0.02</v>
+      </c>
+      <c r="C3" s="37">
+        <v>90.24</v>
+      </c>
+      <c r="D3" s="37">
+        <v>358.93</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B4" s="38">
+        <v>4.7999999999999994E-2</v>
+      </c>
+      <c r="C4" s="39">
+        <v>100.95</v>
+      </c>
+      <c r="D4" s="39">
+        <v>363.82</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B5" s="36">
+        <v>0.10349999999999999</v>
+      </c>
+      <c r="C5" s="37">
+        <v>111.66</v>
+      </c>
+      <c r="D5" s="37">
+        <v>368.75</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B6" s="38">
+        <v>0.2044</v>
+      </c>
+      <c r="C6" s="39">
+        <v>122.36</v>
+      </c>
+      <c r="D6" s="39">
+        <v>373.68</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B7" s="36">
+        <v>0.37470000000000003</v>
+      </c>
+      <c r="C7" s="37">
+        <v>133.11000000000001</v>
+      </c>
+      <c r="D7" s="37">
+        <v>378.58</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B8" s="38">
+        <v>0.64490000000000003</v>
+      </c>
+      <c r="C8" s="39">
+        <v>143.91</v>
+      </c>
+      <c r="D8" s="39">
+        <v>383.39</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B9" s="36">
+        <v>0.71400000000000008</v>
+      </c>
+      <c r="C9" s="37">
+        <v>146.08000000000001</v>
+      </c>
+      <c r="D9" s="37">
+        <v>384.35</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B10" s="38">
+        <v>0.78899999999999992</v>
+      </c>
+      <c r="C10" s="39">
+        <v>148.25</v>
+      </c>
+      <c r="D10" s="39">
+        <v>385.29</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B11" s="36">
+        <v>0.86999999999999988</v>
+      </c>
+      <c r="C11" s="37">
+        <v>150.43</v>
+      </c>
+      <c r="D11" s="37">
+        <v>386.23</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B12" s="38">
+        <v>0.95750000000000002</v>
+      </c>
+      <c r="C12" s="39">
+        <v>152.61000000000001</v>
+      </c>
+      <c r="D12" s="39">
+        <v>387.17</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B13" s="36">
+        <v>1.0131999999999999</v>
+      </c>
+      <c r="C13" s="37">
+        <v>153.93</v>
+      </c>
+      <c r="D13" s="37">
+        <v>387.72</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B14" s="38">
+        <v>1.0518000000000001</v>
+      </c>
+      <c r="C14" s="39">
+        <v>154.80000000000001</v>
+      </c>
+      <c r="D14" s="39">
+        <v>388.09</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B15" s="36">
+        <v>1.1533</v>
+      </c>
+      <c r="C15" s="37">
+        <v>156.99</v>
+      </c>
+      <c r="D15" s="37">
+        <v>389.01</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B16" s="38">
+        <v>1.2623000000000002</v>
+      </c>
+      <c r="C16" s="39">
+        <v>159.19</v>
+      </c>
+      <c r="D16" s="39">
+        <v>389.93</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B17" s="36">
+        <v>1.3793</v>
+      </c>
+      <c r="C17" s="37">
+        <v>161.4</v>
+      </c>
+      <c r="D17" s="37">
+        <v>390.84</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B18" s="38">
+        <v>1.5044999999999999</v>
+      </c>
+      <c r="C18" s="39">
+        <v>163.61000000000001</v>
+      </c>
+      <c r="D18" s="39">
+        <v>391.74</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B19" s="36">
+        <v>1.6384000000000001</v>
+      </c>
+      <c r="C19" s="37">
+        <v>165.82</v>
+      </c>
+      <c r="D19" s="37">
+        <v>392.63</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B20" s="38">
+        <v>1.7815000000000001</v>
+      </c>
+      <c r="C20" s="39">
+        <v>168.04</v>
+      </c>
+      <c r="D20" s="39">
+        <v>393.52</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B21" s="36">
+        <v>1.9339999999999999</v>
+      </c>
+      <c r="C21" s="37">
+        <v>170.27</v>
+      </c>
+      <c r="D21" s="37">
+        <v>394.39</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B22" s="38">
+        <v>2.0964999999999998</v>
+      </c>
+      <c r="C22" s="39">
+        <v>172.51</v>
+      </c>
+      <c r="D22" s="39">
+        <v>395.26</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B23" s="36">
+        <v>2.2692999999999999</v>
+      </c>
+      <c r="C23" s="37">
+        <v>174.75</v>
+      </c>
+      <c r="D23" s="37">
+        <v>396.12</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B24" s="38">
+        <v>2.4529000000000001</v>
+      </c>
+      <c r="C24" s="39">
+        <v>177</v>
+      </c>
+      <c r="D24" s="39">
+        <v>396.67</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B25" s="36">
+        <v>2.6476999999999999</v>
+      </c>
+      <c r="C25" s="37">
+        <v>179.26</v>
+      </c>
+      <c r="D25" s="37">
+        <v>397.81</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B26" s="38">
+        <v>2.8542000000000001</v>
+      </c>
+      <c r="C26" s="39">
+        <v>181.53</v>
+      </c>
+      <c r="D26" s="39">
+        <v>398.64</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B27" s="36">
+        <v>3.0728</v>
+      </c>
+      <c r="C27" s="37">
+        <v>183.81</v>
+      </c>
+      <c r="D27" s="37">
+        <v>399.46</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B28" s="38">
+        <v>3.3040000000000003</v>
+      </c>
+      <c r="C28" s="39">
+        <v>186.09</v>
+      </c>
+      <c r="D28" s="39">
+        <v>400.27</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B29" s="36">
+        <v>3.5482000000000005</v>
+      </c>
+      <c r="C29" s="37">
+        <v>188.38</v>
+      </c>
+      <c r="D29" s="37">
+        <v>401.07</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B30" s="38">
+        <v>3.8058999999999998</v>
+      </c>
+      <c r="C30" s="39">
+        <v>190.69</v>
+      </c>
+      <c r="D30" s="39">
+        <v>401.85</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B31" s="36">
+        <v>4.0774999999999997</v>
+      </c>
+      <c r="C31" s="37">
+        <v>193</v>
+      </c>
+      <c r="D31" s="37">
+        <v>402.63</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B32" s="38">
+        <v>4.3635999999999999</v>
+      </c>
+      <c r="C32" s="39">
+        <v>195.32</v>
+      </c>
+      <c r="D32" s="39">
+        <v>403.39</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B33" s="36">
+        <v>4.6646000000000001</v>
+      </c>
+      <c r="C33" s="37">
+        <v>197.66</v>
+      </c>
+      <c r="D33" s="37">
+        <v>404.14</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B34" s="43">
+        <v>4.9810999999999996</v>
+      </c>
+      <c r="C34" s="44">
+        <v>200</v>
+      </c>
+      <c r="D34" s="44">
+        <v>404.87</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B35" s="36">
+        <v>5.3134000000000006</v>
+      </c>
+      <c r="C35" s="37">
+        <v>202.35</v>
+      </c>
+      <c r="D35" s="37">
+        <v>405.59</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B36" s="38">
+        <v>5.6621999999999995</v>
+      </c>
+      <c r="C36" s="39">
+        <v>204.72</v>
+      </c>
+      <c r="D36" s="39">
+        <v>406.3</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B37" s="36">
+        <v>6.0279000000000007</v>
+      </c>
+      <c r="C37" s="37">
+        <v>207.1</v>
+      </c>
+      <c r="D37" s="37">
+        <v>406.99</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B38" s="38">
+        <v>6.4109000000000007</v>
+      </c>
+      <c r="C38" s="39">
+        <v>209.49</v>
+      </c>
+      <c r="D38" s="39">
+        <v>407.67</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B39" s="36">
+        <v>6.8118999999999996</v>
+      </c>
+      <c r="C39" s="37">
+        <v>211.89</v>
+      </c>
+      <c r="D39" s="37">
+        <v>408.33</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B40" s="38">
+        <v>7.2313999999999998</v>
+      </c>
+      <c r="C40" s="39">
+        <v>214.31</v>
+      </c>
+      <c r="D40" s="39">
+        <v>408.97</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B41" s="36">
+        <v>7.6698000000000004</v>
+      </c>
+      <c r="C41" s="37">
+        <v>216.74</v>
+      </c>
+      <c r="D41" s="37">
+        <v>409.6</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B42" s="38">
+        <v>8.1277000000000008</v>
+      </c>
+      <c r="C42" s="39">
+        <v>219.18</v>
+      </c>
+      <c r="D42" s="39">
+        <v>410.21</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B43" s="36">
+        <v>8.605599999999999</v>
+      </c>
+      <c r="C43" s="37">
+        <v>221.63</v>
+      </c>
+      <c r="D43" s="37">
+        <v>410.8</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B44" s="38">
+        <v>9.1041000000000007</v>
+      </c>
+      <c r="C44" s="39">
+        <v>224.1</v>
+      </c>
+      <c r="D44" s="39">
+        <v>411.38</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B45" s="36">
+        <v>9.6235999999999997</v>
+      </c>
+      <c r="C45" s="37">
+        <v>226.59</v>
+      </c>
+      <c r="D45" s="37">
+        <v>411.93</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B46" s="38">
+        <v>10.164999999999999</v>
+      </c>
+      <c r="C46" s="39">
+        <v>229.09</v>
+      </c>
+      <c r="D46" s="39">
+        <v>412.46</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B47" s="36">
+        <v>10.728</v>
+      </c>
+      <c r="C47" s="37">
+        <v>231.6</v>
+      </c>
+      <c r="D47" s="37">
+        <v>412.98</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B48" s="38">
+        <v>11.314</v>
+      </c>
+      <c r="C48" s="39">
+        <v>234.14</v>
+      </c>
+      <c r="D48" s="39">
+        <v>413.46</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B49" s="36">
+        <v>11.923999999999999</v>
+      </c>
+      <c r="C49" s="37">
+        <v>236.69</v>
+      </c>
+      <c r="D49" s="37">
+        <v>413.93</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B50" s="38">
+        <v>12.557</v>
+      </c>
+      <c r="C50" s="39">
+        <v>239.25</v>
+      </c>
+      <c r="D50" s="39">
+        <v>414.37</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B51" s="36">
+        <v>13.215</v>
+      </c>
+      <c r="C51" s="37">
+        <v>241.84</v>
+      </c>
+      <c r="D51" s="37">
+        <v>414.79</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B52" s="38">
+        <v>13.898</v>
+      </c>
+      <c r="C52" s="39">
+        <v>244.44</v>
+      </c>
+      <c r="D52" s="39">
+        <v>415.18</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B53" s="36">
+        <v>14.605999999999998</v>
+      </c>
+      <c r="C53" s="37">
+        <v>247.06</v>
+      </c>
+      <c r="D53" s="37">
+        <v>415.54</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B54" s="38">
+        <v>15.341000000000001</v>
+      </c>
+      <c r="C54" s="39">
+        <v>249.71</v>
+      </c>
+      <c r="D54" s="39">
+        <v>415.87</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B55" s="36">
+        <v>16.103000000000002</v>
+      </c>
+      <c r="C55" s="37">
+        <v>252.37</v>
+      </c>
+      <c r="D55" s="37">
+        <v>416.17</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B56" s="38">
+        <v>16.891999999999999</v>
+      </c>
+      <c r="C56" s="39">
+        <v>255.06</v>
+      </c>
+      <c r="D56" s="39">
+        <v>416.44</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B57" s="36">
+        <v>17.709</v>
+      </c>
+      <c r="C57" s="37">
+        <v>257.77</v>
+      </c>
+      <c r="D57" s="37">
+        <v>416.68</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B58" s="38">
+        <v>18.555</v>
+      </c>
+      <c r="C58" s="39">
+        <v>260.51</v>
+      </c>
+      <c r="D58" s="39">
+        <v>416.87</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B59" s="36">
+        <v>19.431000000000001</v>
+      </c>
+      <c r="C59" s="37">
+        <v>263.27</v>
+      </c>
+      <c r="D59" s="37">
+        <v>417.03</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B60" s="38">
+        <v>21.753</v>
+      </c>
+      <c r="C60" s="39">
+        <v>270.31</v>
+      </c>
+      <c r="D60" s="39">
+        <v>417.24</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B61" s="36">
+        <v>24.274000000000001</v>
+      </c>
+      <c r="C61" s="37">
+        <v>277.56</v>
+      </c>
+      <c r="D61" s="37">
+        <v>417.14</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B62" s="38">
+        <v>27.008000000000003</v>
+      </c>
+      <c r="C62" s="39">
+        <v>285.06</v>
+      </c>
+      <c r="D62" s="39">
+        <v>416.65</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B63" s="36">
+        <v>29.967000000000002</v>
+      </c>
+      <c r="C63" s="37">
+        <v>292.89999999999998</v>
+      </c>
+      <c r="D63" s="37">
+        <v>415.69</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B64" s="38">
+        <v>33.167999999999999</v>
+      </c>
+      <c r="C64" s="39">
+        <v>301.18</v>
+      </c>
+      <c r="D64" s="39">
+        <v>414.09</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B65" s="36">
+        <v>36.627000000000002</v>
+      </c>
+      <c r="C65" s="37">
+        <v>310.10000000000002</v>
+      </c>
+      <c r="D65" s="37">
+        <v>411.6</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B66" s="38">
+        <v>40.368000000000002</v>
+      </c>
+      <c r="C66" s="39">
+        <v>320.05</v>
+      </c>
+      <c r="D66" s="39">
+        <v>407.72</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B67" s="36">
+        <v>44.416000000000004</v>
+      </c>
+      <c r="C67" s="37">
+        <v>331.98</v>
+      </c>
+      <c r="D67" s="37">
+        <v>401.33</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B68" s="38">
+        <v>48.819999999999993</v>
+      </c>
+      <c r="C68" s="39">
+        <v>348.86</v>
+      </c>
+      <c r="D68" s="39">
+        <v>387.46</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B69" s="40">
+        <v>49.900000000000006</v>
+      </c>
+      <c r="C69" s="41">
+        <v>366.59</v>
+      </c>
+      <c r="D69" s="41">
+        <v>366.59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="182" orientation="portrait" verticalDpi="597" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>